<commit_message>
Updated data dictionary to corrospond with latest diagram
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden\Desktop\Polytech Work\DB2-Design-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9603450-EBF6-47DD-9208-2614011DDFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3CAB77-380A-430B-B182-3DB3FC182682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" firstSheet="5" activeTab="17" xr2:uid="{52EDD9C1-9136-4973-976C-EC648C585359}"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="6" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Role_Category" sheetId="38" r:id="rId5"/>
     <sheet name="Event_Booking" sheetId="39" r:id="rId6"/>
     <sheet name="Field" sheetId="40" r:id="rId7"/>
-    <sheet name="Match_Official" sheetId="41" r:id="rId8"/>
+    <sheet name="Referee" sheetId="41" r:id="rId8"/>
     <sheet name="Incident_report" sheetId="42" r:id="rId9"/>
     <sheet name="Player" sheetId="43" r:id="rId10"/>
     <sheet name="Team" sheetId="44" r:id="rId11"/>
     <sheet name="Match" sheetId="45" r:id="rId12"/>
-    <sheet name="MO_Selection" sheetId="46" r:id="rId13"/>
+    <sheet name="Referee_Selection" sheetId="46" r:id="rId13"/>
     <sheet name="Injury_code" sheetId="47" r:id="rId14"/>
     <sheet name="Player_Team" sheetId="48" r:id="rId15"/>
     <sheet name="Team_Entry" sheetId="49" r:id="rId16"/>
@@ -33,9 +33,8 @@
     <sheet name="Competition" sheetId="51" r:id="rId18"/>
     <sheet name="Position" sheetId="52" r:id="rId19"/>
     <sheet name="Point" sheetId="53" r:id="rId20"/>
-    <sheet name="Result" sheetId="54" r:id="rId21"/>
-    <sheet name="Season" sheetId="55" r:id="rId22"/>
-    <sheet name="Grade" sheetId="56" r:id="rId23"/>
+    <sheet name="Grade" sheetId="56" r:id="rId21"/>
+    <sheet name="Contact" sheetId="58" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="180">
   <si>
     <t>Field Name</t>
   </si>
@@ -121,9 +120,6 @@
     <t>FK</t>
   </si>
   <si>
-    <t>The contact number for the facility</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -160,9 +156,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>unique</t>
-  </si>
-  <si>
     <t>Attributes</t>
   </si>
   <si>
@@ -175,12 +168,6 @@
     <t>address_id</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>An ID that links the a facilities address</t>
-  </si>
-  <si>
     <t>The name of the facility</t>
   </si>
   <si>
@@ -292,12 +279,6 @@
     <t>An ID unique to each address</t>
   </si>
   <si>
-    <t>match_official</t>
-  </si>
-  <si>
-    <t>official_id</t>
-  </si>
-  <si>
     <t>total_games</t>
   </si>
   <si>
@@ -373,27 +354,9 @@
     <t>founded</t>
   </si>
   <si>
-    <t>address_1</t>
-  </si>
-  <si>
-    <t>address_2</t>
-  </si>
-  <si>
     <t>When the team was founded</t>
   </si>
   <si>
-    <t>First line of the teams address</t>
-  </si>
-  <si>
-    <t>Second line of the teams address</t>
-  </si>
-  <si>
-    <t>The city the team is located in</t>
-  </si>
-  <si>
-    <t>The contact number for the team</t>
-  </si>
-  <si>
     <t>First line of the address</t>
   </si>
   <si>
@@ -421,12 +384,6 @@
     <t>An ID which refers to a match</t>
   </si>
   <si>
-    <t>An ID which refers to an official</t>
-  </si>
-  <si>
-    <t>mo_secletion</t>
-  </si>
-  <si>
     <t>code_id</t>
   </si>
   <si>
@@ -511,9 +468,6 @@
     <t>The name/title of the competition</t>
   </si>
   <si>
-    <t>The price(s) for the competition winner(s)</t>
-  </si>
-  <si>
     <t>position</t>
   </si>
   <si>
@@ -529,60 +483,21 @@
     <t>point</t>
   </si>
   <si>
-    <t>result_id</t>
-  </si>
-  <si>
     <t>An ID which refers to a player</t>
   </si>
   <si>
-    <t>An ID which refers to the results</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>season_id</t>
-  </si>
-  <si>
-    <t>An ID unique to each games results</t>
-  </si>
-  <si>
-    <t>An ID which refers to the season the game was played in</t>
-  </si>
-  <si>
     <t>season</t>
   </si>
   <si>
-    <t>winning_team</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
-    <t>final_score</t>
-  </si>
-  <si>
-    <t>The winning team of the season</t>
-  </si>
-  <si>
-    <t>The year which the season took place</t>
-  </si>
-  <si>
     <t>grade</t>
   </si>
   <si>
     <t>grade_id</t>
   </si>
   <si>
-    <t>grade_season</t>
-  </si>
-  <si>
-    <t>grade_comp</t>
-  </si>
-  <si>
     <t>min_dob</t>
   </si>
   <si>
@@ -613,10 +528,73 @@
     <t>An ID which refers to the persons address information</t>
   </si>
   <si>
-    <t>The persons contact email</t>
-  </si>
-  <si>
-    <t>The persons contact mobile number</t>
+    <t>A point scored by a player</t>
+  </si>
+  <si>
+    <t>join_date</t>
+  </si>
+  <si>
+    <t>The date the player joined the team</t>
+  </si>
+  <si>
+    <t>contact_id</t>
+  </si>
+  <si>
+    <t>An ID which refers to the teams address</t>
+  </si>
+  <si>
+    <t>An ID which refers to the teams grade</t>
+  </si>
+  <si>
+    <t>An ID which refers to the teams contact information</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>The final score of the match</t>
+  </si>
+  <si>
+    <t>referee_secletion</t>
+  </si>
+  <si>
+    <t>referee_id</t>
+  </si>
+  <si>
+    <t>An ID which refers to a referee</t>
+  </si>
+  <si>
+    <t>Referee</t>
+  </si>
+  <si>
+    <t>The date which the person started the role</t>
+  </si>
+  <si>
+    <t>An ID which refers to the persons contact information</t>
+  </si>
+  <si>
+    <t>An ID unique to each set of contact information</t>
+  </si>
+  <si>
+    <t>A persons contact email</t>
+  </si>
+  <si>
+    <t>A persons contact mobile</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>An ID which refers the facilities contact information</t>
+  </si>
+  <si>
+    <t>An ID which refers the facilities address</t>
+  </si>
+  <si>
+    <t>The prize(s) for the competition winner(s)</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1101,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1116,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1147,7 +1125,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1159,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1167,10 +1145,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>7</v>
@@ -1183,10 +1161,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1196,10 +1174,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -1209,10 +1187,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1221,44 +1199,36 @@
         <v>20</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>180</v>
+        <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>186</v>
-      </c>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1305,7 +1275,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1289,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1328,7 +1298,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1340,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1348,10 +1318,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>3</v>
@@ -1359,41 +1329,43 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1462,7 +1434,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,13 +1442,13 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1485,7 +1457,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1497,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1505,96 +1477,86 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1641,7 +1603,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1617,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1664,7 +1626,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1676,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1684,10 +1646,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>19</v>
@@ -1699,13 +1661,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1714,21 +1676,27 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1796,12 +1764,12 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
@@ -1810,7 +1778,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1819,7 +1787,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1831,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1839,13 +1807,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -1854,13 +1822,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -1957,7 +1925,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1966,7 +1934,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -1978,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1986,39 +1954,39 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -2094,7 +2062,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,7 +2076,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2117,7 +2085,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2129,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2137,13 +2105,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -2152,36 +2120,42 @@
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2249,7 +2223,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,7 +2237,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2272,7 +2246,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2284,7 +2258,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2292,13 +2266,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -2307,13 +2281,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -2322,13 +2296,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -2404,7 +2378,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,7 +2392,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2427,7 +2401,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2439,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2447,13 +2421,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -2462,13 +2436,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -2550,8 +2524,8 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,7 +2539,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2574,7 +2548,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2586,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2594,46 +2568,50 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="9"/>
     </row>
@@ -2716,7 +2694,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2725,7 +2703,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2737,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2745,39 +2723,39 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -2853,7 +2831,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,13 +2839,13 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2876,7 +2854,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -2888,7 +2866,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2896,26 +2874,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -2924,30 +2902,30 @@
         <v>20</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="B6" s="9" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -3014,7 +2992,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,7 +3006,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3037,7 +3015,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -3049,65 +3027,57 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>160</v>
-      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3170,487 +3140,8 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A655F7D-A785-4C93-BC06-420EDFBA04E5}">
-  <sheetPr codeName="Sheet21"/>
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04E0BCD-1A6F-4935-A798-52EEF861BBCC}">
-  <sheetPr codeName="Sheet22"/>
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92AA4EF-BD71-485B-BCED-5421BE5D232D}">
   <sheetPr codeName="Sheet23"/>
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B497D195-D97D-43BA-A6DB-DEB9A38F07E4}">
-  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3668,7 +3159,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3677,7 +3168,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -3689,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -3697,13 +3188,328 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63FF4AD-6EBB-4D5D-B48E-D66BC4263F8E}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>160</v>
+      </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>77</v>
+        <v>172</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B497D195-D97D-43BA-A6DB-DEB9A38F07E4}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -3713,10 +3519,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -3726,10 +3532,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -3739,23 +3545,23 @@
         <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -3817,7 +3623,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3831,7 +3637,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3840,7 +3646,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -3852,7 +3658,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -3860,13 +3666,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -3875,23 +3681,27 @@
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>170</v>
+      </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3980,7 +3790,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3989,7 +3799,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -4001,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -4009,26 +3819,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -4125,7 +3935,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4134,7 +3944,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -4146,7 +3956,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -4154,10 +3964,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>17</v>
@@ -4169,13 +3979,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -4184,52 +3994,52 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E8" s="10"/>
     </row>
@@ -4298,7 +4108,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4307,7 +4117,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -4319,7 +4129,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -4327,13 +4137,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -4342,39 +4152,39 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -4443,7 +4253,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4457,7 +4267,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4466,7 +4276,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -4478,7 +4288,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -4486,10 +4296,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>16</v>
@@ -4501,26 +4311,26 @@
         <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -4610,7 +4420,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4619,7 +4429,7 @@
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -4631,7 +4441,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -4639,13 +4449,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -4654,54 +4464,54 @@
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="E7" s="9"/>
     </row>

</xml_diff>